<commit_message>
correct expected result file for test 016
</commit_message>
<xml_diff>
--- a/tests/integration/data/Renderer016-ForEach-merged-pyramid/expected.xlsx
+++ b/tests/integration/data/Renderer016-ForEach-merged-pyramid/expected.xlsx
@@ -14,55 +14,76 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
-  <si>
-    <t>col1</t>
-  </si>
-  <si>
-    <t>col2</t>
-  </si>
-  <si>
-    <t>col1 value</t>
-  </si>
-  <si>
-    <t>col1 r2 value</t>
-  </si>
-  <si>
-    <t>col1 r3 value</t>
-  </si>
-  <si>
-    <t>col1 r4 value</t>
-  </si>
-  <si>
-    <t>Second table</t>
-  </si>
-  <si>
-    <t>t2 c1 r1 value</t>
-  </si>
-  <si>
-    <t>t2 c1 r2 value</t>
-  </si>
-  <si>
-    <t>t2 c1 r3 value</t>
-  </si>
-  <si>
-    <t>t2 c1 r4 value</t>
-  </si>
-  <si>
-    <t>After foreach:</t>
-  </si>
-  <si>
-    <t>some value</t>
-  </si>
-  <si>
-    <t>some data</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+  <si>
+    <t>2 items</t>
+  </si>
+  <si>
+    <t>value1 set1</t>
+  </si>
+  <si>
+    <t>1-1</t>
+  </si>
+  <si>
+    <t>value2 set1</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>3 items</t>
+  </si>
+  <si>
+    <t>value1 set2</t>
+  </si>
+  <si>
+    <t>2-1</t>
+  </si>
+  <si>
+    <t>value2 set2</t>
+  </si>
+  <si>
+    <t>2-2</t>
+  </si>
+  <si>
+    <t>value3 set2</t>
+  </si>
+  <si>
+    <t>2-3</t>
+  </si>
+  <si>
+    <t>4 items</t>
+  </si>
+  <si>
+    <t>value1 set3</t>
+  </si>
+  <si>
+    <t>3-1</t>
+  </si>
+  <si>
+    <t>value2 set3</t>
+  </si>
+  <si>
+    <t>3-2</t>
+  </si>
+  <si>
+    <t>value3 set3</t>
+  </si>
+  <si>
+    <t>3-3</t>
+  </si>
+  <si>
+    <t>value4 set3</t>
+  </si>
+  <si>
+    <t>3-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <color theme="1"/>
       <family val="2"/>
@@ -70,17 +91,8 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
-    <font>
-      <b/>
-      <charset val="204"/>
-      <color theme="1"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,13 +101,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.7999816888943144"/>
+        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.7999816888943144"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.5999938962981048"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.1499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -107,17 +131,44 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.3999755851924192"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.7999816888943144"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.3999755851924192"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -135,28 +186,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
@@ -484,136 +559,229 @@
     <col min="1" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4">
+        <v>123</v>
+      </c>
+      <c r="G2" s="4"/>
+      <c r="H2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="4">
+        <v>234</v>
+      </c>
+      <c r="G3" s="4"/>
+      <c r="H3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="2">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2">
+      <c r="G5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="2">
         <v>234</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="2">
+      <c r="G6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="2">
         <v>345</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2">
+      <c r="G7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="8"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="10"/>
+      <c r="F9" s="11">
+        <v>123</v>
+      </c>
+      <c r="G9" s="11"/>
+      <c r="H9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11">
+        <v>234</v>
+      </c>
+      <c r="G10" s="11"/>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11">
+        <v>345</v>
+      </c>
+      <c r="G11" s="11"/>
+      <c r="H11" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="11">
         <v>456</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="7">
-        <v>123</v>
-      </c>
-      <c r="C9" s="7"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="7">
-        <v>234</v>
-      </c>
-      <c r="C10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>345</v>
-      </c>
-      <c r="C11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="7">
-        <v>456</v>
-      </c>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
+  <mergeCells count="28">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="A4:H4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>